<commit_message>
Mise à jour User_Stories
ajout de la méthode jouer()
</commit_message>
<xml_diff>
--- a/Fichiers complémentaires/User_Stories.xlsx
+++ b/Fichiers complémentaires/User_Stories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29780" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>User Story</t>
   </si>
@@ -45,35 +45,301 @@
     <t>En tant qu'utilisateur, j'aimerais pouvoir voir mes vies restantes.</t>
   </si>
   <si>
-    <t>•Créer la classe Joueur, réalisé par
-•Créer la méthode pointVie(), réalisé par</t>
-  </si>
-  <si>
-    <t>•Créer la classe Lettre, réalisé par
-•Créer la méthode verifierLettre(), réalisé par
-•Créer la méthode verifierLettreDansMot(String mot), réalisé par</t>
-  </si>
-  <si>
-    <t>•Créer la classe Dictionnaire, réalisé par
-•Créer la méthode ajouterMot(String mot), réalisé par
-•Créer la méthode supprimerMot(String mot), réalisé par
-•Créer la méthode verifierMotAjout(String mot), réalisé par
-•Créer la méthode verifierMotSuppr(String mot), réalisé par</t>
-  </si>
-  <si>
-    <t>•Créer la classe PenduConsole, réalisé par
-•Créer la méthode menu(), réalisé par
-•Créer la méthode afficherMot(), réalisé par</t>
-  </si>
-  <si>
     <t>En tant qu'utilisateur, j'aimerais avoir un menu pour naviguer.</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">•Créer la classe Joueur, réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nassim</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode pointVie(), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nassim</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">•Créer la classe Lettre, réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nassim</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode verifierLettre(), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nassim</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode verifierLettreDansMot(String mot), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nassim</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">•Créer la classe Dictionnaire, réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sébastien</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode ajouterMot(String mot), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sébastien</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode supprimerMot(String mot), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sébastien</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode verifierMotAjout(String mot), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sébastien</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode verifierMotSuppr(String mot), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sébastien</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">•Créer la classe PenduConsole, réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jean-Eudes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode menu(), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Allaoua</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode afficherMot(), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jean-Eudes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+•Créer la méthode jouer(), réalisé par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Allaoua &amp; Jean-Eudes</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,6 +370,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,12 +453,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -193,6 +461,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -531,13 +805,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="57.5" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -560,60 +834,74 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="116" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="47" customHeight="1" thickBot="1">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="47" customHeight="1" thickBot="1">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="83" customHeight="1" thickBot="1">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="53" customHeight="1" thickBot="1">
-      <c r="A6" s="7">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>